<commit_message>
Re-gen MDS with Stress Monitoring
</commit_message>
<xml_diff>
--- a/output/cooc_questionaire.xlsx
+++ b/output/cooc_questionaire.xlsx
@@ -429,22 +429,22 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.2035882862040077</v>
+        <v>0.2013582225080341</v>
       </c>
       <c r="D2">
-        <v>0.240659839133823</v>
+        <v>0.2333163773956504</v>
       </c>
       <c r="E2">
-        <v>0.4566193717590945</v>
+        <v>0.4564820952209243</v>
       </c>
       <c r="F2">
-        <v>0.3454060483881363</v>
+        <v>0.346880430367577</v>
       </c>
       <c r="G2">
-        <v>0.4410604321250707</v>
+        <v>0.4385702984231664</v>
       </c>
       <c r="H2">
-        <v>0.3226627283946691</v>
+        <v>0.3249153431110011</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -452,25 +452,25 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.2035882862040077</v>
+        <v>0.2013582225080341</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0.182183908520421</v>
+        <v>0.1788672370654924</v>
       </c>
       <c r="E3">
-        <v>0.4404390859660074</v>
+        <v>0.429672575826602</v>
       </c>
       <c r="F3">
-        <v>0.3254194251745592</v>
+        <v>0.3275712988552347</v>
       </c>
       <c r="G3">
-        <v>0.4773927054885804</v>
+        <v>0.4706396546313344</v>
       </c>
       <c r="H3">
-        <v>0.3277714476832352</v>
+        <v>0.3283993633665939</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -478,25 +478,25 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.240659839133823</v>
+        <v>0.2333163773956504</v>
       </c>
       <c r="C4">
-        <v>0.182183908520421</v>
+        <v>0.1788672370654924</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0.4723400979227469</v>
+        <v>0.464145664093723</v>
       </c>
       <c r="F4">
-        <v>0.327421520148345</v>
+        <v>0.3209117648019807</v>
       </c>
       <c r="G4">
-        <v>0.4704925042189136</v>
+        <v>0.4678895691545143</v>
       </c>
       <c r="H4">
-        <v>0.3120528070848201</v>
+        <v>0.3069243545134991</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -504,25 +504,25 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.4566193717590945</v>
+        <v>0.4564820952209243</v>
       </c>
       <c r="C5">
-        <v>0.4404390859660074</v>
+        <v>0.429672575826602</v>
       </c>
       <c r="D5">
-        <v>0.4723400979227469</v>
+        <v>0.464145664093723</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.2657853696474776</v>
+        <v>0.2590022844278493</v>
       </c>
       <c r="G5">
-        <v>0.337278898603976</v>
+        <v>0.3403533178805759</v>
       </c>
       <c r="H5">
-        <v>0.4002650876217305</v>
+        <v>0.3960987825108018</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -530,25 +530,25 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.3454060483881363</v>
+        <v>0.346880430367577</v>
       </c>
       <c r="C6">
-        <v>0.3254194251745592</v>
+        <v>0.3275712988552347</v>
       </c>
       <c r="D6">
-        <v>0.327421520148345</v>
+        <v>0.3209117648019807</v>
       </c>
       <c r="E6">
-        <v>0.2657853696474776</v>
+        <v>0.2590022844278493</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0.3391884542014572</v>
+        <v>0.3253573968246197</v>
       </c>
       <c r="H6">
-        <v>0.2332179651941035</v>
+        <v>0.2378227310462223</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -556,25 +556,25 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.4410604321250707</v>
+        <v>0.4385702984231664</v>
       </c>
       <c r="C7">
-        <v>0.4773927054885804</v>
+        <v>0.4706396546313344</v>
       </c>
       <c r="D7">
-        <v>0.4704925042189136</v>
+        <v>0.4678895691545143</v>
       </c>
       <c r="E7">
-        <v>0.337278898603976</v>
+        <v>0.3403533178805759</v>
       </c>
       <c r="F7">
-        <v>0.3391884542014572</v>
+        <v>0.3253573968246197</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>0.4063847402023144</v>
+        <v>0.3956867380715692</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -582,22 +582,22 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.3226627283946691</v>
+        <v>0.3249153431110011</v>
       </c>
       <c r="C8">
-        <v>0.3277714476832352</v>
+        <v>0.3283993633665939</v>
       </c>
       <c r="D8">
-        <v>0.3120528070848201</v>
+        <v>0.3069243545134991</v>
       </c>
       <c r="E8">
-        <v>0.4002650876217305</v>
+        <v>0.3960987825108018</v>
       </c>
       <c r="F8">
-        <v>0.2332179651941035</v>
+        <v>0.2378227310462223</v>
       </c>
       <c r="G8">
-        <v>0.4063847402023144</v>
+        <v>0.3956867380715692</v>
       </c>
       <c r="H8">
         <v>0</v>

</xml_diff>